<commit_message>
arquivos 1: tunning de modelos aprendizado
</commit_message>
<xml_diff>
--- a/3_Trabalho_Final/resultados/resultados_ensemble.xlsx
+++ b/3_Trabalho_Final/resultados/resultados_ensemble.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statphd-my.sharepoint.com/personal/dionisioneto_statphd_onmicrosoft_com/Documents/Doutorado em Estatística/2023.2/2 - Aprendizado de Máquina Estatístico/3_Trabalho_Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statphd-my.sharepoint.com/personal/dionisioneto_statphd_onmicrosoft_com/Documents/Doutorado em Estatística/2023.2/2 - Aprendizado de Máquina Estatístico/Codigos_Pratica/3_Trabalho_Final/resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FFB08A6-C908-43FF-B473-78D8F1E2FE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{6FFB08A6-C908-43FF-B473-78D8F1E2FE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{557FB8FC-B70B-4AA9-8447-0D46AEF794EA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EEB047B-C8DC-4D6F-96E7-554F48347427}"/>
+    <workbookView xWindow="19090" yWindow="390" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{5EEB047B-C8DC-4D6F-96E7-554F48347427}"/>
   </bookViews>
   <sheets>
     <sheet name="resultados" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>re</t>
   </si>
@@ -93,10 +93,19 @@
     <t>Number os estimators, Number of features, Sample Size</t>
   </si>
   <si>
-    <t>Number of features</t>
-  </si>
-  <si>
     <t>Gráfico de linhas para o k-fold cross validation para cada modelo tunado</t>
+  </si>
+  <si>
+    <t>Cost (Regularization Parameter): it controls the trade-off between having a smooth decision boundary and classifying the training points correctly. A smaller C encourages a wider margin, potentially allowing more training points to be misclassified but promoting a simpler model. A larger C penalizes misclassifications more, resulting in a more complex model. 
+Kernel function: The kernel function determines the type of funtion to be applied in the covariates. Common choices include linear, polynomial, radial basis function (RBF), and sigmoid kernels. The choice of kernel depends genuinely on the characteristics of the data.
+Gamma (Kernel Coefficient for RBF): It defines how far the influence of a single training example reaches. A small gamma will create a more generalized decision boundary, meaning a far reach, while a large gamma will create a more intricate boundary that may fit the training data more closely.
+Epsilon: this hyperparameter is used to control the width of the margin. It defines a margin of tolerance where no penalty is given to errors, allowing some flexibility in fitting the data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ntree: number of trees in the forest. Increasing the number of trees generally improves performance, but it comes at the cost of increased computational complexity. 
+mtry: The number of features to consider when looking for the best split at each node. It can be an integer (representing the exact number of features) or a float (representing a percentage of features).
+Smaller values can reduce overfitting, while larger values may capture more information from the data.
+maxnodes: The minimum number of samples required to split an internal node. Increasing this value can lead to a more conservative model, preventing splits that only capture noise. </t>
   </si>
 </sst>
 </file>
@@ -248,9 +257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>451211</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>3019</xdr:rowOff>
+      <xdr:colOff>453751</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3844769</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -585,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BF8496-5023-4807-B4D2-3075E664EEC2}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +678,7 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -698,14 +707,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D871C4-89D6-42E4-8773-0C1673939BC2}">
   <dimension ref="C2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.3">
@@ -746,18 +755,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:4" ht="316.8" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="3:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kfold para ML - DONE
</commit_message>
<xml_diff>
--- a/3_Trabalho_Final/resultados/resultados_ensemble.xlsx
+++ b/3_Trabalho_Final/resultados/resultados_ensemble.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statphd-my.sharepoint.com/personal/dionisioneto_statphd_onmicrosoft_com/Documents/Doutorado em Estatística/2023.2/2 - Aprendizado de Máquina Estatístico/Codigos_Pratica/3_Trabalho_Final/resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{6FFB08A6-C908-43FF-B473-78D8F1E2FE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{557FB8FC-B70B-4AA9-8447-0D46AEF794EA}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{6FFB08A6-C908-43FF-B473-78D8F1E2FE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9751ABDC-7330-4337-8A91-873D7FF3F8C0}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="390" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{5EEB047B-C8DC-4D6F-96E7-554F48347427}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EEB047B-C8DC-4D6F-96E7-554F48347427}"/>
   </bookViews>
   <sheets>
     <sheet name="resultados" sheetId="1" r:id="rId1"/>
@@ -112,16 +112,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -149,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -160,7 +155,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -293,6 +289,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BF8496-5023-4807-B4D2-3075E664EEC2}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,21 +638,32 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="5">
+        <v>5.6794900000000002E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>5.5655879999999998E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="4">
+        <v>7.4602870000000002E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.3723207</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -707,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D871C4-89D6-42E4-8773-0C1673939BC2}">
   <dimension ref="C2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>